<commit_message>
docs: updated GANTT and IPA-Bericht
</commit_message>
<xml_diff>
--- a/GANTT-Probe-IPA.xlsx
+++ b/GANTT-Probe-IPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasch\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D83BFD6-39A3-4F51-A31F-E1CFBA9D3271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C282620-BF8A-4ADB-9A67-500006FB6C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15720" tabRatio="301" xr2:uid="{D0457A5B-BEB6-4342-89E0-306910FA78BD}"/>
   </bookViews>
@@ -68,12 +68,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Aufbau Dokumentation</t>
-  </si>
-  <si>
-    <t>Grobe Version des Zeitplanes erstellen</t>
-  </si>
-  <si>
     <t>Expertenbesuche</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
   </si>
   <si>
     <t>Projektaufbauorganigram bauen</t>
-  </si>
-  <si>
-    <t>Dokumentation (inklusive Arbeitsjournal)</t>
   </si>
   <si>
     <t>SMART Ziele erstellen</t>
@@ -157,12 +148,21 @@
   <si>
     <t xml:space="preserve">Vorbereitungsphase </t>
   </si>
+  <si>
+    <t>Arbeitsjournal</t>
+  </si>
+  <si>
+    <t>Zeitplan bis und mit [Planen]</t>
+  </si>
+  <si>
+    <t>Zeitplan bis Ende</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +206,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -239,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -687,6 +693,19 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -765,60 +784,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -840,82 +805,49 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -935,6 +867,93 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1255,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5422DD43-1B04-4267-99AB-5339C18D9C14}">
-  <dimension ref="A1:AV58"/>
+  <dimension ref="A1:AV55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1276,158 +1295,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="24" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="24" t="s">
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="24" t="s">
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="24" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="24" t="s">
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="24" t="s">
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="24" t="s">
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="24" t="s">
+      <c r="AD1" s="55"/>
+      <c r="AE1" s="55"/>
+      <c r="AF1" s="56"/>
+      <c r="AG1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="24" t="s">
+      <c r="AH1" s="55"/>
+      <c r="AI1" s="55"/>
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="26"/>
-      <c r="AO1" s="24" t="s">
+      <c r="AL1" s="55"/>
+      <c r="AM1" s="55"/>
+      <c r="AN1" s="56"/>
+      <c r="AO1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="AP1" s="25"/>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="26"/>
-      <c r="AS1" s="24" t="s">
+      <c r="AP1" s="55"/>
+      <c r="AQ1" s="55"/>
+      <c r="AR1" s="56"/>
+      <c r="AS1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="AT1" s="25"/>
-      <c r="AU1" s="25"/>
-      <c r="AV1" s="26"/>
+      <c r="AT1" s="55"/>
+      <c r="AU1" s="55"/>
+      <c r="AV1" s="56"/>
     </row>
     <row r="2" spans="1:48" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="33"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="27">
+      <c r="A2" s="71"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="54">
         <v>45217</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="27">
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="54">
         <v>45222</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="27">
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="54">
         <v>45224</v>
       </c>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="27">
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="54">
         <v>45225</v>
       </c>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="27">
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="54">
         <v>45226</v>
       </c>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="27">
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="54">
         <v>45231</v>
       </c>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="29"/>
-      <c r="AC2" s="27">
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="54">
         <v>45232</v>
       </c>
-      <c r="AD2" s="28"/>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="29"/>
-      <c r="AG2" s="27">
+      <c r="AD2" s="61"/>
+      <c r="AE2" s="61"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="54">
         <v>45233</v>
       </c>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="27">
+      <c r="AH2" s="61"/>
+      <c r="AI2" s="61"/>
+      <c r="AJ2" s="62"/>
+      <c r="AK2" s="54">
         <v>45236</v>
       </c>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="29"/>
-      <c r="AO2" s="27">
+      <c r="AL2" s="61"/>
+      <c r="AM2" s="61"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="54">
         <v>45238</v>
       </c>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
-      <c r="AR2" s="26"/>
-      <c r="AS2" s="27">
+      <c r="AP2" s="55"/>
+      <c r="AQ2" s="55"/>
+      <c r="AR2" s="56"/>
+      <c r="AS2" s="54">
         <v>45239</v>
       </c>
-      <c r="AT2" s="25"/>
-      <c r="AU2" s="25"/>
-      <c r="AV2" s="26"/>
+      <c r="AT2" s="55"/>
+      <c r="AU2" s="55"/>
+      <c r="AV2" s="56"/>
     </row>
     <row r="3" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34"/>
-      <c r="B3" s="37"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
@@ -1568,77 +1587,77 @@
       </c>
     </row>
     <row r="4" spans="1:48" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="30">
-        <v>12</v>
-      </c>
-      <c r="D4" s="30">
+      <c r="A4" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="53">
+        <v>8</v>
+      </c>
+      <c r="D4" s="53">
         <v>0</v>
       </c>
-      <c r="E4" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="15"/>
+      <c r="E4" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="47"/>
+      <c r="G4" s="80"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
       <c r="P4" s="15"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
       <c r="T4" s="15"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="67"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="39"/>
       <c r="X4" s="15"/>
-      <c r="Y4" s="67"/>
-      <c r="Z4" s="67"/>
-      <c r="AA4" s="67"/>
+      <c r="Y4" s="39"/>
+      <c r="Z4" s="39"/>
+      <c r="AA4" s="39"/>
       <c r="AB4" s="15"/>
-      <c r="AC4" s="67"/>
-      <c r="AD4" s="67"/>
-      <c r="AE4" s="67"/>
+      <c r="AC4" s="39"/>
+      <c r="AD4" s="39"/>
+      <c r="AE4" s="39"/>
       <c r="AF4" s="15"/>
-      <c r="AG4" s="67"/>
-      <c r="AH4" s="67"/>
-      <c r="AI4" s="67"/>
+      <c r="AG4" s="39"/>
+      <c r="AH4" s="39"/>
+      <c r="AI4" s="39"/>
       <c r="AJ4" s="15"/>
-      <c r="AK4" s="67"/>
-      <c r="AL4" s="67"/>
-      <c r="AM4" s="67"/>
+      <c r="AK4" s="39"/>
+      <c r="AL4" s="39"/>
+      <c r="AM4" s="39"/>
       <c r="AN4" s="15"/>
-      <c r="AO4" s="67"/>
-      <c r="AP4" s="67"/>
-      <c r="AQ4" s="15"/>
+      <c r="AO4" s="39"/>
+      <c r="AP4" s="39"/>
+      <c r="AQ4" s="80"/>
       <c r="AR4" s="15"/>
-      <c r="AS4" s="15"/>
+      <c r="AS4" s="80"/>
       <c r="AT4" s="15"/>
-      <c r="AU4" s="42"/>
-      <c r="AV4" s="42"/>
+      <c r="AU4" s="24"/>
+      <c r="AV4" s="24"/>
     </row>
     <row r="5" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="69"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="78"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
       <c r="G5" s="16"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
       <c r="L5" s="17"/>
       <c r="M5" s="10"/>
       <c r="N5" s="6"/>
@@ -1675,24 +1694,24 @@
       <c r="AS5" s="10"/>
       <c r="AT5" s="6"/>
       <c r="AU5" s="18"/>
-      <c r="AV5" s="43"/>
+      <c r="AV5" s="25"/>
     </row>
     <row r="6" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="69"/>
-      <c r="B6" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="30">
+      <c r="A6" s="45"/>
+      <c r="B6" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="53">
         <v>2</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="60">
         <v>2</v>
       </c>
-      <c r="E6" s="77"/>
-      <c r="F6" s="78"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="49"/>
       <c r="G6" s="20"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="10"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="22"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="7"/>
@@ -1731,18 +1750,18 @@
       <c r="AS6" s="10"/>
       <c r="AT6" s="6"/>
       <c r="AU6" s="18"/>
-      <c r="AV6" s="43"/>
+      <c r="AV6" s="25"/>
     </row>
     <row r="7" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="69"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="78"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="49"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="10"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="16"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="7"/>
@@ -1781,30 +1800,30 @@
       <c r="AS7" s="10"/>
       <c r="AT7" s="6"/>
       <c r="AU7" s="18"/>
-      <c r="AV7" s="43"/>
+      <c r="AV7" s="25"/>
     </row>
     <row r="8" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69"/>
-      <c r="B8" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="30">
+      <c r="A8" s="45"/>
+      <c r="B8" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="53">
         <v>2</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="53">
         <v>2</v>
       </c>
-      <c r="E8" s="77"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="46"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="28"/>
       <c r="K8" s="6"/>
       <c r="L8" s="7"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="6"/>
@@ -1837,20 +1856,20 @@
       <c r="AS8" s="10"/>
       <c r="AT8" s="6"/>
       <c r="AU8" s="18"/>
-      <c r="AV8" s="43"/>
+      <c r="AV8" s="25"/>
     </row>
     <row r="9" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="69"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="45"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="27"/>
       <c r="L9" s="7"/>
       <c r="M9" s="10"/>
       <c r="N9" s="6"/>
@@ -1887,29 +1906,25 @@
       <c r="AS9" s="10"/>
       <c r="AT9" s="6"/>
       <c r="AU9" s="18"/>
-      <c r="AV9" s="43"/>
-    </row>
-    <row r="10" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="69"/>
-      <c r="B10" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="30">
-        <v>1</v>
-      </c>
-      <c r="D10" s="31">
-        <v>0</v>
-      </c>
-      <c r="E10" s="77"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="6"/>
+      <c r="AV9" s="25"/>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A10" s="45"/>
+      <c r="B10" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="79"/>
       <c r="H10" s="7"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="47"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="78"/>
       <c r="L10" s="7"/>
       <c r="M10" s="10"/>
       <c r="N10" s="20"/>
-      <c r="O10" s="6"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="6"/>
@@ -1942,23 +1957,22 @@
       <c r="AS10" s="10"/>
       <c r="AT10" s="6"/>
       <c r="AU10" s="18"/>
-      <c r="AV10" s="43"/>
+      <c r="AV10" s="25"/>
     </row>
     <row r="11" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="69"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="6"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="79"/>
       <c r="H11" s="7"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="6"/>
+      <c r="J11" s="77"/>
       <c r="K11" s="6"/>
       <c r="L11" s="7"/>
       <c r="M11" s="10"/>
-      <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="10"/>
@@ -1992,29 +2006,30 @@
       <c r="AS11" s="10"/>
       <c r="AT11" s="6"/>
       <c r="AU11" s="18"/>
-      <c r="AV11" s="43"/>
+      <c r="AV11" s="25"/>
     </row>
     <row r="12" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="69"/>
-      <c r="B12" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="56">
-        <v>1</v>
-      </c>
-      <c r="D12" s="56">
+      <c r="A12" s="45"/>
+      <c r="B12" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="53">
+        <v>2</v>
+      </c>
+      <c r="D12" s="60">
         <v>0</v>
       </c>
-      <c r="E12" s="77"/>
-      <c r="F12" s="78"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="49"/>
       <c r="G12" s="6"/>
       <c r="H12" s="7"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="46"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="6"/>
       <c r="L12" s="7"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="20"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="6"/>
@@ -2047,20 +2062,20 @@
       <c r="AS12" s="10"/>
       <c r="AT12" s="6"/>
       <c r="AU12" s="18"/>
-      <c r="AV12" s="43"/>
+      <c r="AV12" s="25"/>
     </row>
     <row r="13" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="69"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="78"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="49"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7"/>
       <c r="I13" s="10"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="45"/>
+      <c r="K13" s="6"/>
       <c r="L13" s="7"/>
       <c r="M13" s="10"/>
       <c r="N13" s="6"/>
@@ -2097,21 +2112,21 @@
       <c r="AS13" s="10"/>
       <c r="AT13" s="6"/>
       <c r="AU13" s="18"/>
-      <c r="AV13" s="43"/>
-    </row>
-    <row r="14" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="69"/>
-      <c r="B14" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="30">
-        <v>6</v>
-      </c>
-      <c r="D14" s="30">
-        <v>3</v>
-      </c>
-      <c r="E14" s="77"/>
-      <c r="F14" s="78"/>
+      <c r="AV13" s="25"/>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A14" s="45"/>
+      <c r="B14" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="58">
+        <v>1</v>
+      </c>
+      <c r="D14" s="58">
+        <v>0</v>
+      </c>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
       <c r="G14" s="6"/>
       <c r="H14" s="7"/>
       <c r="I14" s="22"/>
@@ -2119,7 +2134,6 @@
       <c r="K14" s="20"/>
       <c r="L14" s="21"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="10"/>
@@ -2153,20 +2167,20 @@
       <c r="AS14" s="10"/>
       <c r="AT14" s="6"/>
       <c r="AU14" s="18"/>
-      <c r="AV14" s="43"/>
+      <c r="AV14" s="25"/>
     </row>
     <row r="15" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="69"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="78"/>
+      <c r="A15" s="45"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
       <c r="G15" s="6"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="74"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="41"/>
       <c r="L15" s="17"/>
       <c r="M15" s="10"/>
       <c r="N15" s="6"/>
@@ -2203,30 +2217,31 @@
       <c r="AS15" s="10"/>
       <c r="AT15" s="6"/>
       <c r="AU15" s="18"/>
-      <c r="AV15" s="43"/>
+      <c r="AV15" s="25"/>
     </row>
     <row r="16" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="69"/>
-      <c r="B16" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="30">
-        <v>2</v>
-      </c>
-      <c r="D16" s="31">
-        <v>0</v>
-      </c>
-      <c r="E16" s="77"/>
-      <c r="F16" s="78"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="53">
+        <v>6</v>
+      </c>
+      <c r="D16" s="53">
+        <v>3</v>
+      </c>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49"/>
       <c r="G16" s="6"/>
       <c r="H16" s="7"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="50"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
       <c r="L16" s="21"/>
       <c r="M16" s="20"/>
       <c r="N16" s="6"/>
-      <c r="O16" s="50"/>
-      <c r="P16" s="50"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="7"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
@@ -2258,15 +2273,15 @@
       <c r="AS16" s="10"/>
       <c r="AT16" s="6"/>
       <c r="AU16" s="18"/>
-      <c r="AV16" s="43"/>
+      <c r="AV16" s="25"/>
     </row>
     <row r="17" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="71"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="78"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
       <c r="G17" s="6"/>
       <c r="H17" s="7"/>
       <c r="I17" s="10"/>
@@ -2308,33 +2323,29 @@
       <c r="AS17" s="10"/>
       <c r="AT17" s="6"/>
       <c r="AU17" s="18"/>
-      <c r="AV17" s="43"/>
+      <c r="AV17" s="25"/>
     </row>
     <row r="18" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="30">
+      <c r="A18" s="45"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53">
         <v>2</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="60">
         <v>0</v>
       </c>
-      <c r="E18" s="77"/>
-      <c r="F18" s="78"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
       <c r="G18" s="6"/>
       <c r="H18" s="7"/>
       <c r="I18" s="10"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="23"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
       <c r="M18" s="10"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
-      <c r="P18" s="7"/>
+      <c r="P18" s="6"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
@@ -2366,21 +2377,21 @@
       <c r="AS18" s="10"/>
       <c r="AT18" s="6"/>
       <c r="AU18" s="18"/>
-      <c r="AV18" s="43"/>
+      <c r="AV18" s="25"/>
     </row>
     <row r="19" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="68"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="78"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="49"/>
       <c r="G19" s="6"/>
       <c r="H19" s="7"/>
       <c r="I19" s="10"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-      <c r="L19" s="17"/>
+      <c r="L19" s="6"/>
       <c r="M19" s="10"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
@@ -2416,30 +2427,30 @@
       <c r="AS19" s="10"/>
       <c r="AT19" s="6"/>
       <c r="AU19" s="18"/>
-      <c r="AV19" s="43"/>
+      <c r="AV19" s="25"/>
     </row>
     <row r="20" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="68"/>
-      <c r="B20" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="30">
+      <c r="A20" s="45"/>
+      <c r="B20" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="53">
         <v>2</v>
       </c>
-      <c r="D20" s="31">
-        <v>0</v>
-      </c>
-      <c r="E20" s="77"/>
-      <c r="F20" s="78"/>
+      <c r="D20" s="53">
+        <v>2</v>
+      </c>
+      <c r="E20" s="48"/>
+      <c r="F20" s="49"/>
       <c r="G20" s="6"/>
       <c r="H20" s="7"/>
       <c r="I20" s="10"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="45"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
       <c r="P20" s="7"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="6"/>
@@ -2472,24 +2483,24 @@
       <c r="AS20" s="10"/>
       <c r="AT20" s="6"/>
       <c r="AU20" s="18"/>
-      <c r="AV20" s="43"/>
+      <c r="AV20" s="25"/>
     </row>
     <row r="21" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="68"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="78"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="49"/>
       <c r="G21" s="6"/>
       <c r="H21" s="7"/>
       <c r="I21" s="10"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="62"/>
-      <c r="M21" s="45"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="75"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="45"/>
+      <c r="O21" s="6"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="10"/>
       <c r="R21" s="6"/>
@@ -2522,30 +2533,31 @@
       <c r="AS21" s="10"/>
       <c r="AT21" s="6"/>
       <c r="AU21" s="18"/>
-      <c r="AV21" s="43"/>
+      <c r="AV21" s="25"/>
     </row>
     <row r="22" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="68"/>
-      <c r="B22" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="30">
+      <c r="A22" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="53">
         <v>2</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="60">
         <v>0</v>
       </c>
-      <c r="E22" s="77"/>
-      <c r="F22" s="78"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="49"/>
       <c r="G22" s="6"/>
       <c r="H22" s="7"/>
       <c r="I22" s="10"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="62"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="45"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="31"/>
+      <c r="O22" s="20"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="6"/>
@@ -2578,24 +2590,24 @@
       <c r="AS22" s="10"/>
       <c r="AT22" s="6"/>
       <c r="AU22" s="18"/>
-      <c r="AV22" s="43"/>
+      <c r="AV22" s="25"/>
     </row>
     <row r="23" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="68"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="78"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="49"/>
       <c r="G23" s="6"/>
       <c r="H23" s="7"/>
       <c r="I23" s="10"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="45"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="27"/>
       <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
+      <c r="O23" s="27"/>
       <c r="P23" s="7"/>
       <c r="Q23" s="10"/>
       <c r="R23" s="6"/>
@@ -2628,28 +2640,28 @@
       <c r="AS23" s="10"/>
       <c r="AT23" s="6"/>
       <c r="AU23" s="18"/>
-      <c r="AV23" s="43"/>
+      <c r="AV23" s="25"/>
     </row>
     <row r="24" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="68"/>
-      <c r="B24" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="30">
+      <c r="A24" s="42"/>
+      <c r="B24" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="53">
         <v>2</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="53">
         <v>0</v>
       </c>
-      <c r="E24" s="77"/>
-      <c r="F24" s="78"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="49"/>
       <c r="G24" s="6"/>
       <c r="H24" s="7"/>
       <c r="I24" s="10"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="7"/>
-      <c r="N24" s="20"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="31"/>
       <c r="O24" s="20"/>
       <c r="P24" s="7"/>
       <c r="Q24" s="10"/>
@@ -2683,22 +2695,22 @@
       <c r="AS24" s="10"/>
       <c r="AT24" s="6"/>
       <c r="AU24" s="18"/>
-      <c r="AV24" s="43"/>
+      <c r="AV24" s="25"/>
     </row>
     <row r="25" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="68"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="78"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="49"/>
       <c r="G25" s="6"/>
       <c r="H25" s="7"/>
       <c r="I25" s="10"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="7"/>
-      <c r="M25" s="10"/>
+      <c r="M25" s="27"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="7"/>
@@ -2733,28 +2745,28 @@
       <c r="AS25" s="10"/>
       <c r="AT25" s="6"/>
       <c r="AU25" s="18"/>
-      <c r="AV25" s="43"/>
+      <c r="AV25" s="25"/>
     </row>
     <row r="26" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="68"/>
-      <c r="B26" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="30">
+      <c r="A26" s="42"/>
+      <c r="B26" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="53">
         <v>2</v>
       </c>
-      <c r="D26" s="30">
+      <c r="D26" s="60">
         <v>0</v>
       </c>
-      <c r="E26" s="77"/>
-      <c r="F26" s="78"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="49"/>
       <c r="G26" s="6"/>
       <c r="H26" s="7"/>
       <c r="I26" s="10"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="7"/>
-      <c r="M26" s="10"/>
+      <c r="M26" s="76"/>
       <c r="O26" s="20"/>
       <c r="P26" s="20"/>
       <c r="Q26" s="10"/>
@@ -2788,23 +2800,23 @@
       <c r="AS26" s="10"/>
       <c r="AT26" s="6"/>
       <c r="AU26" s="18"/>
-      <c r="AV26" s="43"/>
+      <c r="AV26" s="25"/>
     </row>
     <row r="27" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="68"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="78"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="49"/>
       <c r="G27" s="6"/>
       <c r="H27" s="7"/>
       <c r="I27" s="10"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="7"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="6"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="27"/>
       <c r="O27" s="6"/>
       <c r="P27" s="7"/>
       <c r="Q27" s="10"/>
@@ -2838,21 +2850,21 @@
       <c r="AS27" s="10"/>
       <c r="AT27" s="6"/>
       <c r="AU27" s="18"/>
-      <c r="AV27" s="43"/>
+      <c r="AV27" s="25"/>
     </row>
     <row r="28" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="68"/>
-      <c r="B28" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="30">
+      <c r="A28" s="42"/>
+      <c r="B28" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="53">
         <v>2</v>
       </c>
-      <c r="D28" s="31">
+      <c r="D28" s="53">
         <v>0</v>
       </c>
-      <c r="E28" s="77"/>
-      <c r="F28" s="78"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="49"/>
       <c r="G28" s="6"/>
       <c r="H28" s="7"/>
       <c r="I28" s="10"/>
@@ -2860,11 +2872,10 @@
       <c r="K28" s="6"/>
       <c r="L28" s="7"/>
       <c r="M28" s="10"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="66"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="6"/>
+      <c r="O28" s="73"/>
+      <c r="P28" s="74"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="20"/>
       <c r="S28" s="6"/>
       <c r="T28" s="7"/>
       <c r="U28" s="10"/>
@@ -2894,15 +2905,15 @@
       <c r="AS28" s="10"/>
       <c r="AT28" s="6"/>
       <c r="AU28" s="18"/>
-      <c r="AV28" s="43"/>
+      <c r="AV28" s="25"/>
     </row>
     <row r="29" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="68"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="78"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="49"/>
       <c r="G29" s="6"/>
       <c r="H29" s="7"/>
       <c r="I29" s="10"/>
@@ -2912,8 +2923,8 @@
       <c r="M29" s="10"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
-      <c r="P29" s="62"/>
-      <c r="Q29" s="10"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="27"/>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
       <c r="T29" s="7"/>
@@ -2944,21 +2955,21 @@
       <c r="AS29" s="10"/>
       <c r="AT29" s="6"/>
       <c r="AU29" s="18"/>
-      <c r="AV29" s="43"/>
+      <c r="AV29" s="25"/>
     </row>
     <row r="30" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="68"/>
-      <c r="B30" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="30">
-        <v>4</v>
-      </c>
-      <c r="D30" s="31">
+      <c r="A30" s="42"/>
+      <c r="B30" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="53">
+        <v>2</v>
+      </c>
+      <c r="D30" s="60">
         <v>0</v>
       </c>
-      <c r="E30" s="77"/>
-      <c r="F30" s="78"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="49"/>
       <c r="G30" s="6"/>
       <c r="H30" s="7"/>
       <c r="I30" s="10"/>
@@ -2967,11 +2978,11 @@
       <c r="L30" s="7"/>
       <c r="M30" s="10"/>
       <c r="N30" s="6"/>
-      <c r="O30" s="50"/>
-      <c r="P30" s="50"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="20"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
       <c r="T30" s="7"/>
       <c r="U30" s="10"/>
       <c r="V30" s="6"/>
@@ -3000,15 +3011,15 @@
       <c r="AS30" s="10"/>
       <c r="AT30" s="6"/>
       <c r="AU30" s="18"/>
-      <c r="AV30" s="43"/>
+      <c r="AV30" s="25"/>
     </row>
     <row r="31" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="68"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="78"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="49"/>
       <c r="G31" s="6"/>
       <c r="H31" s="7"/>
       <c r="I31" s="10"/>
@@ -3018,7 +3029,7 @@
       <c r="M31" s="10"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
-      <c r="P31" s="7"/>
+      <c r="P31" s="36"/>
       <c r="Q31" s="10"/>
       <c r="R31" s="6"/>
       <c r="S31" s="6"/>
@@ -3050,21 +3061,21 @@
       <c r="AS31" s="10"/>
       <c r="AT31" s="6"/>
       <c r="AU31" s="18"/>
-      <c r="AV31" s="43"/>
+      <c r="AV31" s="25"/>
     </row>
     <row r="32" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="68"/>
-      <c r="B32" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="30">
-        <v>2</v>
-      </c>
-      <c r="D32" s="30">
+      <c r="A32" s="42"/>
+      <c r="B32" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="53">
+        <v>4</v>
+      </c>
+      <c r="D32" s="60">
         <v>0</v>
       </c>
-      <c r="E32" s="77"/>
-      <c r="F32" s="78"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="49"/>
       <c r="G32" s="6"/>
       <c r="H32" s="7"/>
       <c r="I32" s="10"/>
@@ -3074,11 +3085,11 @@
       <c r="M32" s="10"/>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
-      <c r="P32" s="50"/>
+      <c r="P32" s="6"/>
       <c r="Q32" s="10"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="50"/>
-      <c r="T32" s="21"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="7"/>
       <c r="U32" s="10"/>
       <c r="V32" s="6"/>
       <c r="W32" s="6"/>
@@ -3106,15 +3117,15 @@
       <c r="AS32" s="10"/>
       <c r="AT32" s="6"/>
       <c r="AU32" s="18"/>
-      <c r="AV32" s="43"/>
+      <c r="AV32" s="25"/>
     </row>
     <row r="33" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="55"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="78"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="49"/>
       <c r="G33" s="6"/>
       <c r="H33" s="7"/>
       <c r="I33" s="10"/>
@@ -3156,23 +3167,21 @@
       <c r="AS33" s="10"/>
       <c r="AT33" s="6"/>
       <c r="AU33" s="18"/>
-      <c r="AV33" s="43"/>
+      <c r="AV33" s="25"/>
     </row>
     <row r="34" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="30">
-        <v>4</v>
-      </c>
-      <c r="D34" s="31">
+      <c r="A34" s="42"/>
+      <c r="B34" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="53">
+        <v>2</v>
+      </c>
+      <c r="D34" s="53">
         <v>0</v>
       </c>
-      <c r="E34" s="77"/>
-      <c r="F34" s="78"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="49"/>
       <c r="G34" s="6"/>
       <c r="H34" s="7"/>
       <c r="I34" s="10"/>
@@ -3182,13 +3191,13 @@
       <c r="M34" s="10"/>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="50"/>
-      <c r="R34" s="50"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="6"/>
       <c r="S34" s="6"/>
-      <c r="T34" s="7"/>
-      <c r="U34" s="20"/>
-      <c r="V34" s="20"/>
+      <c r="T34" s="21"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="6"/>
       <c r="W34" s="6"/>
       <c r="X34" s="7"/>
       <c r="Y34" s="10"/>
@@ -3214,15 +3223,15 @@
       <c r="AS34" s="10"/>
       <c r="AT34" s="6"/>
       <c r="AU34" s="18"/>
-      <c r="AV34" s="43"/>
+      <c r="AV34" s="25"/>
     </row>
     <row r="35" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="68"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="78"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="49"/>
       <c r="G35" s="6"/>
       <c r="H35" s="7"/>
       <c r="I35" s="10"/>
@@ -3264,21 +3273,23 @@
       <c r="AS35" s="10"/>
       <c r="AT35" s="6"/>
       <c r="AU35" s="18"/>
-      <c r="AV35" s="43"/>
+      <c r="AV35" s="25"/>
     </row>
     <row r="36" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="68"/>
-      <c r="B36" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="30">
-        <v>8</v>
-      </c>
-      <c r="D36" s="30">
+      <c r="A36" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="53">
+        <v>4</v>
+      </c>
+      <c r="D36" s="60">
         <v>0</v>
       </c>
-      <c r="E36" s="77"/>
-      <c r="F36" s="78"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="49"/>
       <c r="G36" s="6"/>
       <c r="H36" s="7"/>
       <c r="I36" s="10"/>
@@ -3289,15 +3300,16 @@
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="7"/>
-      <c r="Q36" s="10"/>
-      <c r="S36" s="50"/>
-      <c r="T36" s="50"/>
-      <c r="U36" s="10"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="20"/>
-      <c r="X36" s="20"/>
-      <c r="Y36" s="22"/>
-      <c r="Z36" s="20"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="6"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="10"/>
+      <c r="Z36" s="6"/>
       <c r="AA36" s="6"/>
       <c r="AB36" s="7"/>
       <c r="AC36" s="10"/>
@@ -3319,15 +3331,15 @@
       <c r="AS36" s="10"/>
       <c r="AT36" s="6"/>
       <c r="AU36" s="18"/>
-      <c r="AV36" s="43"/>
+      <c r="AV36" s="25"/>
     </row>
     <row r="37" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="68"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="78"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="49"/>
       <c r="G37" s="6"/>
       <c r="H37" s="7"/>
       <c r="I37" s="10"/>
@@ -3342,10 +3354,10 @@
       <c r="R37" s="6"/>
       <c r="S37" s="6"/>
       <c r="T37" s="7"/>
-      <c r="U37" s="50"/>
-      <c r="V37" s="50"/>
-      <c r="W37" s="50"/>
-      <c r="X37" s="50"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="6"/>
+      <c r="W37" s="6"/>
+      <c r="X37" s="7"/>
       <c r="Y37" s="10"/>
       <c r="Z37" s="6"/>
       <c r="AA37" s="6"/>
@@ -3369,21 +3381,21 @@
       <c r="AS37" s="10"/>
       <c r="AT37" s="6"/>
       <c r="AU37" s="18"/>
-      <c r="AV37" s="43"/>
+      <c r="AV37" s="25"/>
     </row>
     <row r="38" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="68"/>
-      <c r="B38" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="30">
-        <v>4</v>
-      </c>
-      <c r="D38" s="30">
+      <c r="A38" s="42"/>
+      <c r="B38" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="53">
+        <v>8</v>
+      </c>
+      <c r="D38" s="53">
         <v>0</v>
       </c>
-      <c r="E38" s="77"/>
-      <c r="F38" s="78"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="49"/>
       <c r="G38" s="6"/>
       <c r="H38" s="7"/>
       <c r="I38" s="10"/>
@@ -3395,17 +3407,16 @@
       <c r="O38" s="6"/>
       <c r="P38" s="7"/>
       <c r="Q38" s="10"/>
-      <c r="R38" s="6"/>
       <c r="S38" s="6"/>
-      <c r="T38" s="7"/>
-      <c r="U38" s="51"/>
-      <c r="V38" s="50"/>
-      <c r="W38" s="50"/>
-      <c r="X38" s="64"/>
-      <c r="Y38" s="10"/>
-      <c r="Z38" s="6"/>
-      <c r="AA38" s="20"/>
-      <c r="AB38" s="21"/>
+      <c r="T38" s="6"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="6"/>
+      <c r="W38" s="20"/>
+      <c r="X38" s="20"/>
+      <c r="Y38" s="22"/>
+      <c r="Z38" s="20"/>
+      <c r="AA38" s="6"/>
+      <c r="AB38" s="7"/>
       <c r="AC38" s="10"/>
       <c r="AD38" s="6"/>
       <c r="AE38" s="6"/>
@@ -3425,15 +3436,15 @@
       <c r="AS38" s="10"/>
       <c r="AT38" s="6"/>
       <c r="AU38" s="18"/>
-      <c r="AV38" s="43"/>
+      <c r="AV38" s="25"/>
     </row>
     <row r="39" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="68"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="78"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="49"/>
       <c r="G39" s="6"/>
       <c r="H39" s="7"/>
       <c r="I39" s="10"/>
@@ -3448,10 +3459,10 @@
       <c r="R39" s="6"/>
       <c r="S39" s="6"/>
       <c r="T39" s="7"/>
-      <c r="U39" s="51"/>
-      <c r="V39" s="50"/>
-      <c r="W39" s="50"/>
-      <c r="X39" s="64"/>
+      <c r="U39" s="6"/>
+      <c r="V39" s="6"/>
+      <c r="W39" s="6"/>
+      <c r="X39" s="6"/>
       <c r="Y39" s="10"/>
       <c r="Z39" s="6"/>
       <c r="AA39" s="6"/>
@@ -3475,21 +3486,21 @@
       <c r="AS39" s="10"/>
       <c r="AT39" s="6"/>
       <c r="AU39" s="18"/>
-      <c r="AV39" s="43"/>
+      <c r="AV39" s="25"/>
     </row>
     <row r="40" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="68"/>
-      <c r="B40" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="30">
-        <v>8</v>
-      </c>
-      <c r="D40" s="31">
+      <c r="A40" s="42"/>
+      <c r="B40" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="53">
+        <v>4</v>
+      </c>
+      <c r="D40" s="53">
         <v>0</v>
       </c>
-      <c r="E40" s="77"/>
-      <c r="F40" s="78"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="49"/>
       <c r="G40" s="6"/>
       <c r="H40" s="7"/>
       <c r="I40" s="10"/>
@@ -3504,17 +3515,18 @@
       <c r="R40" s="6"/>
       <c r="S40" s="6"/>
       <c r="T40" s="7"/>
-      <c r="U40" s="10"/>
+      <c r="U40" s="27"/>
       <c r="V40" s="6"/>
       <c r="W40" s="6"/>
-      <c r="X40" s="7"/>
-      <c r="Y40" s="49"/>
-      <c r="Z40" s="50"/>
-      <c r="AA40" s="46"/>
-      <c r="AC40" s="22"/>
-      <c r="AD40" s="20"/>
-      <c r="AE40" s="20"/>
-      <c r="AF40" s="21"/>
+      <c r="X40" s="37"/>
+      <c r="Y40" s="10"/>
+      <c r="Z40" s="6"/>
+      <c r="AA40" s="20"/>
+      <c r="AB40" s="21"/>
+      <c r="AC40" s="10"/>
+      <c r="AD40" s="6"/>
+      <c r="AE40" s="6"/>
+      <c r="AF40" s="7"/>
       <c r="AG40" s="10"/>
       <c r="AH40" s="6"/>
       <c r="AI40" s="6"/>
@@ -3530,15 +3542,15 @@
       <c r="AS40" s="10"/>
       <c r="AT40" s="6"/>
       <c r="AU40" s="18"/>
-      <c r="AV40" s="43"/>
+      <c r="AV40" s="25"/>
     </row>
     <row r="41" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="68"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="78"/>
+      <c r="A41" s="42"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="49"/>
       <c r="G41" s="6"/>
       <c r="H41" s="7"/>
       <c r="I41" s="10"/>
@@ -3553,15 +3565,15 @@
       <c r="R41" s="6"/>
       <c r="S41" s="6"/>
       <c r="T41" s="7"/>
-      <c r="U41" s="10"/>
+      <c r="U41" s="27"/>
       <c r="V41" s="6"/>
       <c r="W41" s="6"/>
-      <c r="X41" s="7"/>
+      <c r="X41" s="37"/>
       <c r="Y41" s="10"/>
       <c r="Z41" s="6"/>
       <c r="AA41" s="6"/>
-      <c r="AB41" s="62"/>
-      <c r="AC41" s="45"/>
+      <c r="AB41" s="7"/>
+      <c r="AC41" s="10"/>
       <c r="AD41" s="6"/>
       <c r="AE41" s="6"/>
       <c r="AF41" s="7"/>
@@ -3580,21 +3592,21 @@
       <c r="AS41" s="10"/>
       <c r="AT41" s="6"/>
       <c r="AU41" s="18"/>
-      <c r="AV41" s="43"/>
+      <c r="AV41" s="25"/>
     </row>
     <row r="42" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="68"/>
-      <c r="B42" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="C42" s="30">
+      <c r="A42" s="42"/>
+      <c r="B42" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="53">
         <v>8</v>
       </c>
-      <c r="D42" s="30">
+      <c r="D42" s="60">
         <v>0</v>
       </c>
-      <c r="E42" s="77"/>
-      <c r="F42" s="78"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="49"/>
       <c r="G42" s="6"/>
       <c r="H42" s="7"/>
       <c r="I42" s="10"/>
@@ -3615,18 +3627,17 @@
       <c r="X42" s="7"/>
       <c r="Y42" s="10"/>
       <c r="Z42" s="6"/>
-      <c r="AA42" s="6"/>
-      <c r="AB42" s="7"/>
-      <c r="AC42" s="51"/>
-      <c r="AD42" s="6"/>
-      <c r="AE42" s="6"/>
-      <c r="AF42" s="7"/>
-      <c r="AG42" s="52"/>
-      <c r="AH42" s="20"/>
-      <c r="AI42" s="20"/>
-      <c r="AJ42" s="20"/>
-      <c r="AK42" s="49"/>
-      <c r="AL42" s="50"/>
+      <c r="AA42" s="28"/>
+      <c r="AC42" s="22"/>
+      <c r="AD42" s="20"/>
+      <c r="AE42" s="20"/>
+      <c r="AF42" s="21"/>
+      <c r="AG42" s="10"/>
+      <c r="AH42" s="6"/>
+      <c r="AI42" s="6"/>
+      <c r="AJ42" s="7"/>
+      <c r="AK42" s="10"/>
+      <c r="AL42" s="6"/>
       <c r="AM42" s="6"/>
       <c r="AN42" s="7"/>
       <c r="AO42" s="10"/>
@@ -3636,15 +3647,15 @@
       <c r="AS42" s="10"/>
       <c r="AT42" s="6"/>
       <c r="AU42" s="18"/>
-      <c r="AV42" s="43"/>
+      <c r="AV42" s="25"/>
     </row>
     <row r="43" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="68"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="77"/>
-      <c r="F43" s="78"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="49"/>
       <c r="G43" s="6"/>
       <c r="H43" s="7"/>
       <c r="I43" s="10"/>
@@ -3666,12 +3677,12 @@
       <c r="Y43" s="10"/>
       <c r="Z43" s="6"/>
       <c r="AA43" s="6"/>
-      <c r="AB43" s="7"/>
-      <c r="AC43" s="45"/>
+      <c r="AB43" s="36"/>
+      <c r="AC43" s="27"/>
       <c r="AD43" s="6"/>
       <c r="AE43" s="6"/>
       <c r="AF43" s="7"/>
-      <c r="AG43" s="45"/>
+      <c r="AG43" s="10"/>
       <c r="AH43" s="6"/>
       <c r="AI43" s="6"/>
       <c r="AJ43" s="7"/>
@@ -3686,21 +3697,21 @@
       <c r="AS43" s="10"/>
       <c r="AT43" s="6"/>
       <c r="AU43" s="18"/>
-      <c r="AV43" s="43"/>
+      <c r="AV43" s="25"/>
     </row>
     <row r="44" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="68"/>
-      <c r="B44" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="C44" s="56">
+      <c r="A44" s="42"/>
+      <c r="B44" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="53">
         <v>8</v>
       </c>
-      <c r="D44" s="56">
+      <c r="D44" s="53">
         <v>0</v>
       </c>
-      <c r="E44" s="77"/>
-      <c r="F44" s="78"/>
+      <c r="E44" s="48"/>
+      <c r="F44" s="49"/>
       <c r="G44" s="6"/>
       <c r="H44" s="7"/>
       <c r="I44" s="10"/>
@@ -3723,33 +3734,34 @@
       <c r="Z44" s="6"/>
       <c r="AA44" s="6"/>
       <c r="AB44" s="7"/>
-      <c r="AC44" s="45"/>
+      <c r="AC44" s="27"/>
       <c r="AD44" s="6"/>
       <c r="AE44" s="6"/>
       <c r="AF44" s="7"/>
-      <c r="AG44" s="45"/>
-      <c r="AH44" s="6"/>
-      <c r="AI44" s="6"/>
-      <c r="AJ44" s="7"/>
-      <c r="AK44" s="20"/>
-      <c r="AL44" s="20"/>
-      <c r="AM44" s="52"/>
-      <c r="AN44" s="21"/>
-      <c r="AO44" s="65"/>
+      <c r="AG44" s="31"/>
+      <c r="AH44" s="20"/>
+      <c r="AI44" s="20"/>
+      <c r="AJ44" s="20"/>
+      <c r="AK44" s="10"/>
+      <c r="AL44" s="6"/>
+      <c r="AM44" s="6"/>
+      <c r="AN44" s="7"/>
+      <c r="AO44" s="10"/>
+      <c r="AP44" s="6"/>
       <c r="AQ44" s="6"/>
       <c r="AR44" s="7"/>
       <c r="AS44" s="10"/>
       <c r="AT44" s="6"/>
       <c r="AU44" s="18"/>
-      <c r="AV44" s="43"/>
+      <c r="AV44" s="25"/>
     </row>
     <row r="45" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="68"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="77"/>
-      <c r="F45" s="78"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="49"/>
       <c r="G45" s="6"/>
       <c r="H45" s="7"/>
       <c r="I45" s="10"/>
@@ -3772,42 +3784,40 @@
       <c r="Z45" s="6"/>
       <c r="AA45" s="6"/>
       <c r="AB45" s="7"/>
-      <c r="AC45" s="45"/>
+      <c r="AC45" s="27"/>
       <c r="AD45" s="6"/>
       <c r="AE45" s="6"/>
       <c r="AF45" s="7"/>
-      <c r="AG45" s="45"/>
+      <c r="AG45" s="27"/>
       <c r="AH45" s="6"/>
       <c r="AI45" s="6"/>
       <c r="AJ45" s="7"/>
       <c r="AK45" s="10"/>
       <c r="AL45" s="6"/>
-      <c r="AM45" s="45"/>
+      <c r="AM45" s="6"/>
       <c r="AN45" s="7"/>
-      <c r="AO45" s="45"/>
-      <c r="AP45" s="45"/>
+      <c r="AO45" s="10"/>
+      <c r="AP45" s="6"/>
       <c r="AQ45" s="6"/>
       <c r="AR45" s="7"/>
       <c r="AS45" s="10"/>
       <c r="AT45" s="6"/>
       <c r="AU45" s="18"/>
-      <c r="AV45" s="43"/>
+      <c r="AV45" s="25"/>
     </row>
     <row r="46" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" s="30">
-        <v>6</v>
-      </c>
-      <c r="D46" s="31">
+      <c r="A46" s="42"/>
+      <c r="B46" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="58">
+        <v>8</v>
+      </c>
+      <c r="D46" s="58">
         <v>0</v>
       </c>
-      <c r="E46" s="77"/>
-      <c r="F46" s="78"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="49"/>
       <c r="G46" s="6"/>
       <c r="H46" s="7"/>
       <c r="I46" s="10"/>
@@ -3830,34 +3840,33 @@
       <c r="Z46" s="6"/>
       <c r="AA46" s="6"/>
       <c r="AB46" s="7"/>
-      <c r="AC46" s="45"/>
+      <c r="AC46" s="27"/>
       <c r="AD46" s="6"/>
       <c r="AE46" s="6"/>
       <c r="AF46" s="7"/>
-      <c r="AG46" s="45"/>
+      <c r="AG46" s="27"/>
       <c r="AH46" s="6"/>
       <c r="AI46" s="6"/>
       <c r="AJ46" s="7"/>
-      <c r="AK46" s="10"/>
-      <c r="AL46" s="6"/>
-      <c r="AM46" s="6"/>
-      <c r="AN46" s="62"/>
-      <c r="AO46" s="52"/>
-      <c r="AP46" s="52"/>
-      <c r="AQ46" s="52"/>
-      <c r="AR46" s="21"/>
+      <c r="AK46" s="20"/>
+      <c r="AL46" s="20"/>
+      <c r="AM46" s="31"/>
+      <c r="AN46" s="21"/>
+      <c r="AO46" s="38"/>
+      <c r="AQ46" s="6"/>
+      <c r="AR46" s="7"/>
       <c r="AS46" s="10"/>
       <c r="AT46" s="6"/>
       <c r="AU46" s="18"/>
-      <c r="AV46" s="43"/>
+      <c r="AV46" s="25"/>
     </row>
     <row r="47" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="68"/>
-      <c r="B47" s="55"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="78"/>
+      <c r="A47" s="42"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="49"/>
       <c r="G47" s="6"/>
       <c r="H47" s="7"/>
       <c r="I47" s="10"/>
@@ -3880,40 +3889,42 @@
       <c r="Z47" s="6"/>
       <c r="AA47" s="6"/>
       <c r="AB47" s="7"/>
-      <c r="AC47" s="45"/>
+      <c r="AC47" s="27"/>
       <c r="AD47" s="6"/>
       <c r="AE47" s="6"/>
       <c r="AF47" s="7"/>
-      <c r="AG47" s="45"/>
+      <c r="AG47" s="27"/>
       <c r="AH47" s="6"/>
       <c r="AI47" s="6"/>
       <c r="AJ47" s="7"/>
       <c r="AK47" s="10"/>
       <c r="AL47" s="6"/>
-      <c r="AM47" s="6"/>
-      <c r="AN47" s="62"/>
-      <c r="AO47" s="45"/>
-      <c r="AP47" s="45"/>
-      <c r="AQ47" s="45"/>
+      <c r="AM47" s="27"/>
+      <c r="AN47" s="7"/>
+      <c r="AO47" s="27"/>
+      <c r="AP47" s="27"/>
+      <c r="AQ47" s="6"/>
       <c r="AR47" s="7"/>
       <c r="AS47" s="10"/>
       <c r="AT47" s="6"/>
       <c r="AU47" s="18"/>
-      <c r="AV47" s="43"/>
+      <c r="AV47" s="25"/>
     </row>
     <row r="48" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="68"/>
-      <c r="B48" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="C48" s="30">
-        <v>2</v>
-      </c>
-      <c r="D48" s="30">
+      <c r="A48" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="53">
+        <v>6</v>
+      </c>
+      <c r="D48" s="60">
         <v>0</v>
       </c>
-      <c r="E48" s="77"/>
-      <c r="F48" s="78"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="49"/>
       <c r="G48" s="6"/>
       <c r="H48" s="7"/>
       <c r="I48" s="10"/>
@@ -3936,34 +3947,34 @@
       <c r="Z48" s="6"/>
       <c r="AA48" s="6"/>
       <c r="AB48" s="7"/>
-      <c r="AC48" s="45"/>
+      <c r="AC48" s="27"/>
       <c r="AD48" s="6"/>
       <c r="AE48" s="6"/>
       <c r="AF48" s="7"/>
-      <c r="AG48" s="45"/>
+      <c r="AG48" s="27"/>
       <c r="AH48" s="6"/>
       <c r="AI48" s="6"/>
       <c r="AJ48" s="7"/>
       <c r="AK48" s="10"/>
       <c r="AL48" s="6"/>
       <c r="AM48" s="6"/>
-      <c r="AN48" s="62"/>
-      <c r="AO48" s="45"/>
-      <c r="AP48" s="45"/>
-      <c r="AQ48" s="52"/>
+      <c r="AN48" s="36"/>
+      <c r="AO48" s="31"/>
+      <c r="AP48" s="31"/>
+      <c r="AQ48" s="31"/>
       <c r="AR48" s="21"/>
       <c r="AS48" s="10"/>
       <c r="AT48" s="6"/>
       <c r="AU48" s="18"/>
-      <c r="AV48" s="43"/>
+      <c r="AV48" s="25"/>
     </row>
     <row r="49" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="55"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="77"/>
-      <c r="F49" s="78"/>
+      <c r="A49" s="42"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="49"/>
       <c r="G49" s="6"/>
       <c r="H49" s="7"/>
       <c r="I49" s="10"/>
@@ -3986,42 +3997,40 @@
       <c r="Z49" s="6"/>
       <c r="AA49" s="6"/>
       <c r="AB49" s="7"/>
-      <c r="AC49" s="45"/>
+      <c r="AC49" s="27"/>
       <c r="AD49" s="6"/>
       <c r="AE49" s="6"/>
       <c r="AF49" s="7"/>
-      <c r="AG49" s="45"/>
+      <c r="AG49" s="27"/>
       <c r="AH49" s="6"/>
       <c r="AI49" s="6"/>
       <c r="AJ49" s="7"/>
       <c r="AK49" s="10"/>
       <c r="AL49" s="6"/>
       <c r="AM49" s="6"/>
-      <c r="AN49" s="62"/>
-      <c r="AO49" s="45"/>
-      <c r="AP49" s="45"/>
-      <c r="AQ49" s="45"/>
+      <c r="AN49" s="36"/>
+      <c r="AO49" s="27"/>
+      <c r="AP49" s="27"/>
+      <c r="AQ49" s="27"/>
       <c r="AR49" s="7"/>
       <c r="AS49" s="10"/>
       <c r="AT49" s="6"/>
       <c r="AU49" s="18"/>
-      <c r="AV49" s="43"/>
+      <c r="AV49" s="25"/>
     </row>
     <row r="50" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" s="35" t="s">
+      <c r="A50" s="42"/>
+      <c r="B50" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C50" s="30">
-        <v>6</v>
-      </c>
-      <c r="D50" s="31">
+      <c r="C50" s="53">
+        <v>2</v>
+      </c>
+      <c r="D50" s="53">
         <v>0</v>
       </c>
-      <c r="E50" s="77"/>
-      <c r="F50" s="78"/>
+      <c r="E50" s="48"/>
+      <c r="F50" s="49"/>
       <c r="G50" s="6"/>
       <c r="H50" s="7"/>
       <c r="I50" s="10"/>
@@ -4044,120 +4053,271 @@
       <c r="Z50" s="6"/>
       <c r="AA50" s="6"/>
       <c r="AB50" s="7"/>
-      <c r="AC50" s="45"/>
+      <c r="AC50" s="27"/>
       <c r="AD50" s="6"/>
       <c r="AE50" s="6"/>
       <c r="AF50" s="7"/>
-      <c r="AG50" s="10"/>
+      <c r="AG50" s="27"/>
       <c r="AH50" s="6"/>
       <c r="AI50" s="6"/>
       <c r="AJ50" s="7"/>
       <c r="AK50" s="10"/>
       <c r="AL50" s="6"/>
       <c r="AM50" s="6"/>
-      <c r="AN50" s="7"/>
-      <c r="AO50" s="45"/>
-      <c r="AP50" s="45"/>
-      <c r="AQ50" s="52"/>
+      <c r="AN50" s="36"/>
+      <c r="AO50" s="27"/>
+      <c r="AP50" s="27"/>
+      <c r="AQ50" s="31"/>
       <c r="AR50" s="21"/>
-      <c r="AS50" s="22"/>
-      <c r="AT50" s="20"/>
+      <c r="AS50" s="10"/>
+      <c r="AT50" s="6"/>
       <c r="AU50" s="18"/>
-      <c r="AV50" s="43"/>
+      <c r="AV50" s="25"/>
     </row>
     <row r="51" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="55"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="79"/>
-      <c r="F51" s="80"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="9"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="8"/>
-      <c r="O51" s="8"/>
-      <c r="P51" s="9"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="8"/>
-      <c r="S51" s="8"/>
-      <c r="T51" s="9"/>
-      <c r="U51" s="11"/>
-      <c r="V51" s="8"/>
-      <c r="W51" s="8"/>
-      <c r="X51" s="9"/>
-      <c r="Y51" s="11"/>
-      <c r="Z51" s="8"/>
-      <c r="AA51" s="8"/>
-      <c r="AB51" s="9"/>
-      <c r="AC51" s="11"/>
-      <c r="AD51" s="8"/>
-      <c r="AE51" s="8"/>
-      <c r="AF51" s="9"/>
-      <c r="AG51" s="11"/>
-      <c r="AH51" s="8"/>
-      <c r="AI51" s="8"/>
-      <c r="AJ51" s="9"/>
-      <c r="AK51" s="11"/>
-      <c r="AL51" s="8"/>
-      <c r="AM51" s="58"/>
-      <c r="AN51" s="59"/>
-      <c r="AO51" s="60"/>
-      <c r="AP51" s="60"/>
-      <c r="AQ51" s="61"/>
-      <c r="AR51" s="9"/>
-      <c r="AS51" s="11"/>
-      <c r="AT51" s="8"/>
-      <c r="AU51" s="19"/>
-      <c r="AV51" s="44"/>
+      <c r="A51" s="43"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="6"/>
+      <c r="S51" s="6"/>
+      <c r="T51" s="7"/>
+      <c r="U51" s="10"/>
+      <c r="V51" s="6"/>
+      <c r="W51" s="6"/>
+      <c r="X51" s="7"/>
+      <c r="Y51" s="10"/>
+      <c r="Z51" s="6"/>
+      <c r="AA51" s="6"/>
+      <c r="AB51" s="7"/>
+      <c r="AC51" s="27"/>
+      <c r="AD51" s="6"/>
+      <c r="AE51" s="6"/>
+      <c r="AF51" s="7"/>
+      <c r="AG51" s="27"/>
+      <c r="AH51" s="6"/>
+      <c r="AI51" s="6"/>
+      <c r="AJ51" s="7"/>
+      <c r="AK51" s="10"/>
+      <c r="AL51" s="6"/>
+      <c r="AM51" s="6"/>
+      <c r="AN51" s="36"/>
+      <c r="AO51" s="27"/>
+      <c r="AP51" s="27"/>
+      <c r="AQ51" s="27"/>
+      <c r="AR51" s="7"/>
+      <c r="AS51" s="10"/>
+      <c r="AT51" s="6"/>
+      <c r="AU51" s="18"/>
+      <c r="AV51" s="25"/>
     </row>
     <row r="52" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="13" t="s">
+      <c r="A52" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="53">
+        <v>6</v>
+      </c>
+      <c r="D52" s="60">
+        <v>0</v>
+      </c>
+      <c r="E52" s="48"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="10"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+      <c r="P52" s="7"/>
+      <c r="Q52" s="10"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="6"/>
+      <c r="T52" s="7"/>
+      <c r="U52" s="10"/>
+      <c r="V52" s="6"/>
+      <c r="W52" s="6"/>
+      <c r="X52" s="7"/>
+      <c r="Y52" s="10"/>
+      <c r="Z52" s="6"/>
+      <c r="AA52" s="6"/>
+      <c r="AB52" s="7"/>
+      <c r="AC52" s="27"/>
+      <c r="AD52" s="6"/>
+      <c r="AE52" s="6"/>
+      <c r="AF52" s="7"/>
+      <c r="AG52" s="10"/>
+      <c r="AH52" s="6"/>
+      <c r="AI52" s="6"/>
+      <c r="AJ52" s="7"/>
+      <c r="AK52" s="10"/>
+      <c r="AL52" s="6"/>
+      <c r="AM52" s="6"/>
+      <c r="AN52" s="7"/>
+      <c r="AO52" s="27"/>
+      <c r="AP52" s="27"/>
+      <c r="AQ52" s="31"/>
+      <c r="AR52" s="21"/>
+      <c r="AS52" s="22"/>
+      <c r="AT52" s="20"/>
+      <c r="AU52" s="18"/>
+      <c r="AV52" s="25"/>
+    </row>
+    <row r="53" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="43"/>
+      <c r="B53" s="57"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="11"/>
+      <c r="R53" s="8"/>
+      <c r="S53" s="8"/>
+      <c r="T53" s="9"/>
+      <c r="U53" s="11"/>
+      <c r="V53" s="8"/>
+      <c r="W53" s="8"/>
+      <c r="X53" s="9"/>
+      <c r="Y53" s="11"/>
+      <c r="Z53" s="8"/>
+      <c r="AA53" s="8"/>
+      <c r="AB53" s="9"/>
+      <c r="AC53" s="11"/>
+      <c r="AD53" s="8"/>
+      <c r="AE53" s="8"/>
+      <c r="AF53" s="9"/>
+      <c r="AG53" s="11"/>
+      <c r="AH53" s="8"/>
+      <c r="AI53" s="8"/>
+      <c r="AJ53" s="9"/>
+      <c r="AK53" s="11"/>
+      <c r="AL53" s="8"/>
+      <c r="AM53" s="32"/>
+      <c r="AN53" s="33"/>
+      <c r="AO53" s="34"/>
+      <c r="AP53" s="34"/>
+      <c r="AQ53" s="35"/>
+      <c r="AR53" s="9"/>
+      <c r="AS53" s="11"/>
+      <c r="AT53" s="8"/>
+      <c r="AU53" s="19"/>
+      <c r="AV53" s="26"/>
+    </row>
+    <row r="54" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C52" s="14">
-        <f>SUM(C4:C51)</f>
-        <v>98</v>
-      </c>
-      <c r="D52" s="14">
-        <f>SUM(D4:D51)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:48" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="AC55" s="53"/>
-    </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="W58" s="63"/>
-    </row>
+      <c r="C54" s="14">
+        <f>SUM(C4:C53)</f>
+        <v>95</v>
+      </c>
+      <c r="D54" s="14">
+        <f>SUM(D4:D53)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:48" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="103">
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A4:A17"/>
-    <mergeCell ref="E4:F51"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="A34:A45"/>
-    <mergeCell ref="A46:A49"/>
+  <mergeCells count="106">
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="AK2:AN2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AK1:AN1"/>
+    <mergeCell ref="AO1:AR1"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A22:A35"/>
+    <mergeCell ref="A4:A21"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="AS2:AV2"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="C48:C49"/>
     <mergeCell ref="D48:D49"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="AS2:AV2"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
     <mergeCell ref="AG2:AJ2"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="Q2:T2"/>
@@ -4167,79 +4327,33 @@
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="C1:D2"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="E4:F53"/>
+    <mergeCell ref="A36:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
     <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="AS1:AV1"/>
-    <mergeCell ref="AK2:AN2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AK1:AN1"/>
-    <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="AC1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>